<commit_message>
v 1.0.3 (fixed data calculating and readMe.md)
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowHeight="19300"/>
+    <workbookView windowWidth="23660" windowHeight="7300"/>
   </bookViews>
   <sheets>
     <sheet name="Export" sheetId="1" r:id="rId1"/>
@@ -1845,13 +1845,66 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1866,61 +1919,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1942,8 +1941,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1957,22 +1965,22 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1988,22 +1996,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2018,31 +2018,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2060,13 +2042,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2084,7 +2060,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2102,7 +2078,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2114,7 +2090,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2126,25 +2168,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2162,31 +2186,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2198,7 +2198,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2227,26 +2227,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -2258,15 +2238,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2286,15 +2257,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2309,151 +2271,189 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2844,8 +2844,8 @@
   <sheetPr/>
   <dimension ref="A1:U613"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.94117647058824" defaultRowHeight="14.8"/>
@@ -3146,7 +3146,6 @@
       <c r="L5" t="s">
         <v>36</v>
       </c>
-      <c r="M5"/>
       <c r="N5">
         <v>0.4</v>
       </c>
@@ -3209,7 +3208,6 @@
       <c r="L6" t="s">
         <v>37</v>
       </c>
-      <c r="M6"/>
       <c r="N6" t="s">
         <v>32</v>
       </c>
@@ -3523,7 +3521,6 @@
       <c r="L11" t="s">
         <v>43</v>
       </c>
-      <c r="M11"/>
       <c r="N11" t="s">
         <v>32</v>
       </c>

</xml_diff>